<commit_message>
se cambio el driver para el manejo de historias.
</commit_message>
<xml_diff>
--- a/excel/GUI Automated Testing - User registration.xlsx
+++ b/excel/GUI Automated Testing - User registration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" firstSheet="13" activeTab="18"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" firstSheet="15" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="GUI_UR_AP_001" sheetId="1" r:id="rId1"/>
@@ -776,7 +776,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="I14" sqref="A1:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2732,8 +2732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3132,7 +3132,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3154,8 +3154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>